<commit_message>
PCB and Enclosure Update
- Swapped RJ11 connector to match Sparkfun Breakout board / reduce number of parts
- Swapped RJ11 wiring to match QWIIC adapter board / LipSync
- Modified USB Knockout on Case
-
</commit_message>
<xml_diff>
--- a/Documentation/Working_Documents/Forest_Hub_BOM.xlsx
+++ b/Documentation/Working_Documents/Forest_Hub_BOM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://neilsquiresoc.sharepoint.com/sites/MMC-RD/Shared Documents/RD 23-05 ATP Joysticks/Forest Hub/Forest-Joystick-Mouse-Hub/Documentation/Working_Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://neilsquiresoc.sharepoint.com/sites/Jake/Shared Documents/General/GitHub/Forest-Joystick-Mouse-Hub/Documentation/Working_Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="829" documentId="11_DC0E2523FAFE28515E8D5C5A1D4A6B02C3B15AFA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CD2989E2-3377-4A03-98E7-15135A84D690}"/>
+  <xr:revisionPtr revIDLastSave="841" documentId="11_DC0E2523FAFE28515E8D5C5A1D4A6B02C3B15AFA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8546A137-A498-4C5B-A6CC-40647F451BC4}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{248D1F3E-BF0A-44FC-936F-F83C4AA85C2C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="124">
   <si>
     <t>Total Cost</t>
   </si>
@@ -392,10 +392,22 @@
     <t>https://www.mouser.ca/ProductDetail/538-90147-1107</t>
   </si>
   <si>
-    <t>Version: V1.01</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 2023-Oct-13</t>
+    <t>Version: V2.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2023-Nov-25</t>
+  </si>
+  <si>
+    <t>RJ 11 Connector</t>
+  </si>
+  <si>
+    <t>TE Connectivity / AMP</t>
+  </si>
+  <si>
+    <t>571-5555165-1</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/TE-Connectivity-AMP/5555165-1?qs=BcfjnG7NVaWb2UIqidZ6Zg%3D%3D</t>
   </si>
 </sst>
 </file>
@@ -972,10 +984,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8EF84FC-3600-43C4-9213-7FDCEB4DF0DE}">
-  <dimension ref="A1:Q39"/>
+  <dimension ref="A1:Q40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1029,19 +1041,19 @@
       <c r="E2" s="11"/>
       <c r="F2" s="11"/>
       <c r="J2" s="6">
-        <f>SUM(H31:H33)</f>
+        <f>SUM(H32:H34)</f>
         <v>0</v>
       </c>
       <c r="K2" s="24">
-        <f>SUM(K5:K21,K25:K26)</f>
-        <v>55.677999999999997</v>
+        <f>SUM(K5:K22,K26:K27)</f>
+        <v>57.137999999999991</v>
       </c>
       <c r="L2" s="5">
-        <f>SUM(L5:L29)+J34</f>
-        <v>108.90500000000003</v>
+        <f>SUM(L5:L30)+J35</f>
+        <v>110.36500000000001</v>
       </c>
       <c r="M2" s="26">
-        <f>SUM(M31:M33)</f>
+        <f>SUM(M32:M34)</f>
         <v>7.4999999999999997E-2</v>
       </c>
     </row>
@@ -1124,7 +1136,7 @@
         <v>10.88</v>
       </c>
       <c r="K5" s="16">
-        <f t="shared" ref="K5:K20" si="0">IF(G5&gt;0,J5/H5,0)</f>
+        <f t="shared" ref="K5:K21" si="0">IF(G5&gt;0,J5/H5,0)</f>
         <v>10.88</v>
       </c>
       <c r="L5" s="16">
@@ -1158,7 +1170,7 @@
         <v>1</v>
       </c>
       <c r="I6">
-        <f t="shared" ref="I6:I21" si="1">IF(G6&gt;0,CEILING(G6/H6,1),0)</f>
+        <f t="shared" ref="I6:I22" si="1">IF(G6&gt;0,CEILING(G6/H6,1),0)</f>
         <v>2</v>
       </c>
       <c r="J6" s="9">
@@ -1169,7 +1181,7 @@
         <v>3.32</v>
       </c>
       <c r="L6" s="16">
-        <f t="shared" ref="L6:L21" si="2">I6*J6</f>
+        <f t="shared" ref="L6:L22" si="2">I6*J6</f>
         <v>6.64</v>
       </c>
       <c r="N6" s="8" t="s">
@@ -1424,19 +1436,19 @@
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>42</v>
+        <v>120</v>
       </c>
       <c r="C13" t="s">
-        <v>32</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>48</v>
+        <v>68</v>
+      </c>
+      <c r="D13" t="s">
+        <v>121</v>
       </c>
       <c r="E13" t="s">
         <v>19</v>
       </c>
       <c r="F13" s="23" t="s">
-        <v>45</v>
+        <v>122</v>
       </c>
       <c r="G13">
         <v>1</v>
@@ -1449,26 +1461,26 @@
         <v>1</v>
       </c>
       <c r="J13" s="9">
-        <v>0.15</v>
+        <v>1.46</v>
       </c>
       <c r="K13" s="16">
         <f t="shared" si="0"/>
-        <v>0.15</v>
+        <v>1.46</v>
       </c>
       <c r="L13" s="16">
         <f t="shared" si="2"/>
-        <v>0.15</v>
+        <v>1.46</v>
       </c>
       <c r="N13" s="8" t="s">
-        <v>44</v>
+        <v>123</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="C14" t="s">
-        <v>59</v>
+        <v>32</v>
       </c>
       <c r="D14" s="8" t="s">
         <v>48</v>
@@ -1477,7 +1489,7 @@
         <v>19</v>
       </c>
       <c r="F14" s="23" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
       <c r="G14">
         <v>1</v>
@@ -1490,26 +1502,26 @@
         <v>1</v>
       </c>
       <c r="J14" s="9">
-        <v>0.14499999999999999</v>
+        <v>0.15</v>
       </c>
       <c r="K14" s="16">
         <f t="shared" si="0"/>
-        <v>0.14499999999999999</v>
+        <v>0.15</v>
       </c>
       <c r="L14" s="16">
         <f t="shared" si="2"/>
-        <v>0.14499999999999999</v>
+        <v>0.15</v>
       </c>
       <c r="N14" s="8" t="s">
-        <v>61</v>
+        <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D15" s="8" t="s">
         <v>48</v>
@@ -1518,7 +1530,7 @@
         <v>19</v>
       </c>
       <c r="F15" s="23" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G15">
         <v>1</v>
@@ -1542,15 +1554,15 @@
         <v>0.14499999999999999</v>
       </c>
       <c r="N15" s="8" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="C16" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="D16" s="8" t="s">
         <v>48</v>
@@ -1559,17 +1571,17 @@
         <v>19</v>
       </c>
       <c r="F16" s="23" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="G16">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H16">
         <v>1</v>
       </c>
       <c r="I16">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J16" s="9">
         <v>0.14499999999999999</v>
@@ -1580,18 +1592,18 @@
       </c>
       <c r="L16" s="16">
         <f t="shared" si="2"/>
-        <v>0.28999999999999998</v>
+        <v>0.14499999999999999</v>
       </c>
       <c r="N16" s="8" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
     </row>
     <row r="17" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="C17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D17" s="8" t="s">
         <v>48</v>
@@ -1600,17 +1612,17 @@
         <v>19</v>
       </c>
       <c r="F17" s="23" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="G17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H17">
         <v>1</v>
       </c>
       <c r="I17">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J17" s="9">
         <v>0.14499999999999999</v>
@@ -1621,27 +1633,27 @@
       </c>
       <c r="L17" s="16">
         <f t="shared" si="2"/>
-        <v>0.14499999999999999</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="N17" s="8" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
     </row>
     <row r="18" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>78</v>
+        <v>43</v>
       </c>
       <c r="C18" t="s">
-        <v>77</v>
+        <v>58</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>79</v>
+        <v>48</v>
       </c>
       <c r="E18" t="s">
         <v>19</v>
       </c>
       <c r="F18" s="23" t="s">
-        <v>81</v>
+        <v>47</v>
       </c>
       <c r="G18">
         <v>1</v>
@@ -1654,33 +1666,35 @@
         <v>1</v>
       </c>
       <c r="J18" s="9">
-        <v>1</v>
+        <v>0.14499999999999999</v>
       </c>
       <c r="K18" s="16">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.14499999999999999</v>
       </c>
       <c r="L18" s="16">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0.14499999999999999</v>
       </c>
       <c r="N18" s="8" t="s">
-        <v>80</v>
+        <v>46</v>
       </c>
     </row>
     <row r="19" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>106</v>
+        <v>78</v>
       </c>
       <c r="C19" t="s">
-        <v>107</v>
-      </c>
-      <c r="D19" s="8"/>
+        <v>77</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>79</v>
+      </c>
       <c r="E19" t="s">
         <v>19</v>
       </c>
       <c r="F19" s="23" t="s">
-        <v>112</v>
+        <v>81</v>
       </c>
       <c r="G19">
         <v>1</v>
@@ -1693,35 +1707,33 @@
         <v>1</v>
       </c>
       <c r="J19" s="9">
-        <v>0.49</v>
+        <v>1</v>
       </c>
       <c r="K19" s="16">
         <f t="shared" si="0"/>
-        <v>0.49</v>
+        <v>1</v>
       </c>
       <c r="L19" s="16">
         <f t="shared" si="2"/>
-        <v>0.49</v>
+        <v>1</v>
       </c>
       <c r="N19" s="8" t="s">
-        <v>111</v>
+        <v>80</v>
       </c>
     </row>
     <row r="20" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>73</v>
+        <v>106</v>
       </c>
       <c r="C20" t="s">
-        <v>76</v>
-      </c>
-      <c r="D20" s="25" t="s">
-        <v>15</v>
-      </c>
+        <v>107</v>
+      </c>
+      <c r="D20" s="8"/>
       <c r="E20" t="s">
         <v>19</v>
       </c>
       <c r="F20" s="23" t="s">
-        <v>75</v>
+        <v>112</v>
       </c>
       <c r="G20">
         <v>1</v>
@@ -1734,27 +1746,36 @@
         <v>1</v>
       </c>
       <c r="J20" s="9">
-        <v>7.18</v>
+        <v>0.49</v>
       </c>
       <c r="K20" s="16">
         <f t="shared" si="0"/>
-        <v>7.18</v>
+        <v>0.49</v>
       </c>
       <c r="L20" s="16">
         <f t="shared" si="2"/>
-        <v>7.18</v>
+        <v>0.49</v>
       </c>
       <c r="N20" s="8" t="s">
-        <v>74</v>
+        <v>111</v>
       </c>
     </row>
     <row r="21" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>39</v>
+        <v>73</v>
+      </c>
+      <c r="C21" t="s">
+        <v>76</v>
+      </c>
+      <c r="D21" s="25" t="s">
+        <v>15</v>
       </c>
       <c r="E21" t="s">
         <v>19</v>
       </c>
+      <c r="F21" s="23" t="s">
+        <v>75</v>
+      </c>
       <c r="G21">
         <v>1</v>
       </c>
@@ -1765,130 +1786,131 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="J21" s="27">
-        <v>20</v>
+      <c r="J21" s="9">
+        <v>7.18</v>
       </c>
       <c r="K21" s="16">
-        <f>IF(G21&gt;0,J21/H21,0)</f>
-        <v>20</v>
+        <f t="shared" si="0"/>
+        <v>7.18</v>
       </c>
       <c r="L21" s="16">
         <f t="shared" si="2"/>
+        <v>7.18</v>
+      </c>
+      <c r="N21" s="8" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="22" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>39</v>
+      </c>
+      <c r="E22" t="s">
+        <v>19</v>
+      </c>
+      <c r="G22">
+        <v>1</v>
+      </c>
+      <c r="H22">
+        <v>1</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J22" s="27">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J22" s="27"/>
-      <c r="K22" s="30"/>
-      <c r="L22" s="30"/>
-    </row>
-    <row r="23" spans="2:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="14" t="s">
+      <c r="K22" s="16">
+        <f>IF(G22&gt;0,J22/H22,0)</f>
+        <v>20</v>
+      </c>
+      <c r="L22" s="16">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J23" s="27"/>
+      <c r="K23" s="30"/>
+      <c r="L23" s="30"/>
+    </row>
+    <row r="24" spans="2:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="14" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="24" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="7" t="s">
+    <row r="25" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C24" s="7" t="s">
+      <c r="C25" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D24" s="7" t="s">
+      <c r="D25" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="E24" s="7" t="s">
+      <c r="E25" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="F24" s="7" t="s">
+      <c r="F25" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="G24" s="7" t="s">
+      <c r="G25" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="H24" s="7" t="s">
+      <c r="H25" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="I24" s="7" t="s">
+      <c r="I25" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="J24" s="7" t="s">
+      <c r="J25" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="K24" s="15" t="s">
+      <c r="K25" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="L24" s="15" t="s">
+      <c r="L25" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="M24" s="7"/>
-      <c r="N24" s="7" t="s">
+      <c r="M25" s="7"/>
+      <c r="N25" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="Q24" s="8"/>
-    </row>
-    <row r="25" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
-        <v>92</v>
-      </c>
-      <c r="C25" t="s">
-        <v>93</v>
-      </c>
-      <c r="D25" t="s">
-        <v>104</v>
-      </c>
-      <c r="F25" s="23"/>
-      <c r="G25">
-        <v>1</v>
-      </c>
-      <c r="H25">
-        <v>5</v>
-      </c>
-      <c r="I25">
-        <f t="shared" ref="I25:I27" si="3">IF(G25&gt;0,CEILING(G25/H25,1),0)</f>
-        <v>1</v>
-      </c>
-      <c r="J25" s="9">
-        <v>12.26</v>
-      </c>
-      <c r="K25" s="16">
-        <f>IF(G25&gt;0,J25/H25,0)</f>
-        <v>2.452</v>
-      </c>
-      <c r="L25" s="16">
-        <f t="shared" ref="L25:L27" si="4">I25*J25</f>
-        <v>12.26</v>
-      </c>
-      <c r="N25" s="8"/>
+      <c r="Q25" s="8"/>
     </row>
     <row r="26" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C26" t="s">
-        <v>101</v>
+        <v>93</v>
+      </c>
+      <c r="D26" t="s">
+        <v>104</v>
       </c>
       <c r="F26" s="23"/>
       <c r="G26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H26">
         <v>5</v>
       </c>
       <c r="I26">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" ref="I26:I28" si="3">IF(G26&gt;0,CEILING(G26/H26,1),0)</f>
+        <v>1</v>
       </c>
       <c r="J26" s="9">
-        <v>40.33</v>
+        <v>12.26</v>
       </c>
       <c r="K26" s="16">
         <f>IF(G26&gt;0,J26/H26,0)</f>
-        <v>0</v>
+        <v>2.452</v>
       </c>
       <c r="L26" s="16">
-        <f t="shared" si="4"/>
-        <v>0</v>
+        <f t="shared" ref="L26:L28" si="4">I26*J26</f>
+        <v>12.26</v>
       </c>
       <c r="N26" s="8"/>
     </row>
@@ -1897,121 +1919,126 @@
         <v>94</v>
       </c>
       <c r="C27" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F27" s="23"/>
       <c r="G27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H27">
         <v>5</v>
       </c>
       <c r="I27">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J27" s="9">
-        <v>24.07</v>
+        <v>40.33</v>
       </c>
       <c r="K27" s="16">
         <f>IF(G27&gt;0,J27/H27,0)</f>
-        <v>4.8140000000000001</v>
+        <v>0</v>
       </c>
       <c r="L27" s="16">
         <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="N27" s="8"/>
+    </row>
+    <row r="28" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>94</v>
+      </c>
+      <c r="C28" t="s">
+        <v>103</v>
+      </c>
+      <c r="F28" s="23"/>
+      <c r="G28">
+        <v>1</v>
+      </c>
+      <c r="H28">
+        <v>5</v>
+      </c>
+      <c r="I28">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="J28" s="9">
         <v>24.07</v>
       </c>
-      <c r="N27" s="8"/>
-    </row>
-    <row r="28" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C28" s="21"/>
-      <c r="K28" s="17"/>
-      <c r="L28" s="17"/>
+      <c r="K28" s="16">
+        <f>IF(G28&gt;0,J28/H28,0)</f>
+        <v>4.8140000000000001</v>
+      </c>
+      <c r="L28" s="16">
+        <f t="shared" si="4"/>
+        <v>24.07</v>
+      </c>
+      <c r="N28" s="8"/>
     </row>
     <row r="29" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="19" t="s">
+      <c r="C29" s="21"/>
+      <c r="K29" s="17"/>
+      <c r="L29" s="17"/>
+    </row>
+    <row r="30" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C29" s="32">
+      <c r="C30" s="32">
         <v>30</v>
       </c>
-      <c r="J29" s="9"/>
-      <c r="K29" s="18"/>
-      <c r="L29" s="18"/>
-      <c r="M29" s="24"/>
-    </row>
-    <row r="30" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="7" t="s">
+      <c r="J30" s="9"/>
+      <c r="K30" s="18"/>
+      <c r="L30" s="18"/>
+      <c r="M30" s="24"/>
+    </row>
+    <row r="31" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C30" s="20" t="s">
+      <c r="C31" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="D30" s="7"/>
-      <c r="E30" s="7"/>
-      <c r="F30" s="7"/>
-      <c r="G30" s="7" t="s">
+      <c r="D31" s="7"/>
+      <c r="E31" s="7"/>
+      <c r="F31" s="7"/>
+      <c r="G31" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="H30" s="7" t="s">
+      <c r="H31" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="I30" s="15"/>
-      <c r="J30" s="15" t="s">
+      <c r="I31" s="15"/>
+      <c r="J31" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="K30" s="7" t="s">
+      <c r="K31" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="L30" s="7" t="s">
+      <c r="L31" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="M30" s="7" t="s">
+      <c r="M31" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="N30" s="7" t="s">
+      <c r="N31" s="7" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="31" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B31" t="s">
-        <v>85</v>
-      </c>
-      <c r="C31" t="s">
-        <v>87</v>
-      </c>
-      <c r="G31">
-        <v>1</v>
-      </c>
-      <c r="J31" s="16"/>
-      <c r="K31" s="16">
-        <f t="shared" ref="K31:L33" si="5">($H$32/1000)*$C$29</f>
-        <v>0</v>
-      </c>
-      <c r="L31" s="16">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="M31" s="28">
-        <v>2.4999999999999998E-2</v>
       </c>
     </row>
     <row r="32" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C32" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G32">
         <v>1</v>
       </c>
-      <c r="J32" s="16">
-        <f>($H$32/1000)*$C$29</f>
-        <v>0</v>
-      </c>
+      <c r="J32" s="16"/>
       <c r="K32" s="16">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="K32:L34" si="5">($H$33/1000)*$C$30</f>
         <v>0</v>
       </c>
       <c r="L32" s="16">
@@ -2019,24 +2046,21 @@
         <v>0</v>
       </c>
       <c r="M32" s="28">
-        <v>4.9999999999999996E-2</v>
-      </c>
-      <c r="O32" s="10"/>
-      <c r="P32" s="10"/>
-      <c r="Q32" s="10"/>
-    </row>
-    <row r="33" spans="2:14" x14ac:dyDescent="0.25">
+        <v>2.4999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
-        <v>113</v>
+        <v>86</v>
       </c>
       <c r="C33" t="s">
-        <v>114</v>
+        <v>88</v>
       </c>
       <c r="G33">
         <v>1</v>
       </c>
       <c r="J33" s="16">
-        <f>(H33/1000)*$C$29</f>
+        <f>($H$33/1000)*$C$30</f>
         <v>0</v>
       </c>
       <c r="K33" s="16">
@@ -2047,121 +2071,150 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="11"/>
-      <c r="L34" s="12"/>
-    </row>
-    <row r="35" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="31" t="s">
+      <c r="M33" s="28">
+        <v>4.9999999999999996E-2</v>
+      </c>
+      <c r="O33" s="10"/>
+      <c r="P33" s="10"/>
+      <c r="Q33" s="10"/>
+    </row>
+    <row r="34" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>113</v>
+      </c>
+      <c r="C34" t="s">
+        <v>114</v>
+      </c>
+      <c r="G34">
+        <v>1</v>
+      </c>
+      <c r="J34" s="16">
+        <f>(H34/1000)*$C$30</f>
+        <v>0</v>
+      </c>
+      <c r="K34" s="16">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="L34" s="16">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B35" s="11"/>
+      <c r="L35" s="12"/>
+    </row>
+    <row r="36" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B36" s="31" t="s">
         <v>89</v>
       </c>
-      <c r="C35" s="10"/>
-      <c r="D35" s="10"/>
-      <c r="E35" s="10"/>
-      <c r="F35" s="10"/>
-      <c r="G35" s="10"/>
-      <c r="H35" s="10"/>
-      <c r="I35" s="10"/>
-      <c r="J35" s="10"/>
-      <c r="K35" s="10"/>
-      <c r="L35" s="10"/>
-      <c r="M35" s="10"/>
-      <c r="N35" s="10"/>
-    </row>
-    <row r="36" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="22" t="s">
+      <c r="C36" s="10"/>
+      <c r="D36" s="10"/>
+      <c r="E36" s="10"/>
+      <c r="F36" s="10"/>
+      <c r="G36" s="10"/>
+      <c r="H36" s="10"/>
+      <c r="I36" s="10"/>
+      <c r="J36" s="10"/>
+      <c r="K36" s="10"/>
+      <c r="L36" s="10"/>
+      <c r="M36" s="10"/>
+      <c r="N36" s="10"/>
+    </row>
+    <row r="37" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B37" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="C36" s="22" t="s">
+      <c r="C37" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="D36" s="29" t="s">
+      <c r="D37" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="E36" s="29" t="s">
+      <c r="E37" s="29" t="s">
         <v>82</v>
       </c>
-      <c r="F36" s="29"/>
-    </row>
-    <row r="37" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B37" t="s">
+      <c r="F37" s="29"/>
+    </row>
+    <row r="38" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
         <v>108</v>
       </c>
-      <c r="E37" t="s">
+      <c r="E38" t="s">
         <v>109</v>
       </c>
-      <c r="G37">
-        <v>1</v>
-      </c>
-      <c r="H37">
+      <c r="G38">
+        <v>1</v>
+      </c>
+      <c r="H38">
         <v>100</v>
       </c>
-      <c r="I37">
-        <f t="shared" ref="I37:I39" si="6">IF(G37&gt;0,CEILING(G37/H37,1),0)</f>
-        <v>1</v>
-      </c>
-      <c r="J37" s="27">
+      <c r="I38">
+        <f t="shared" ref="I38:I40" si="6">IF(G38&gt;0,CEILING(G38/H38,1),0)</f>
+        <v>1</v>
+      </c>
+      <c r="J38" s="27">
         <v>9.3000000000000007</v>
       </c>
-      <c r="K37" s="16">
-        <f t="shared" ref="K37" si="7">IF(G37&gt;0,J37/H37,0)</f>
+      <c r="K38" s="16">
+        <f t="shared" ref="K38" si="7">IF(G38&gt;0,J38/H38,0)</f>
         <v>9.3000000000000013E-2</v>
       </c>
-      <c r="L37" s="16">
-        <f t="shared" ref="L37" si="8">I37*J37</f>
+      <c r="L38" s="16">
+        <f t="shared" ref="L38" si="8">I38*J38</f>
         <v>9.3000000000000007</v>
       </c>
-      <c r="N37" s="8" t="s">
+      <c r="N38" s="8" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="39" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B39" t="s">
+    <row r="40" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
         <v>14</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C40" t="s">
         <v>90</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D40" t="s">
         <v>15</v>
       </c>
-      <c r="E39" t="s">
+      <c r="E40" t="s">
         <v>19</v>
       </c>
-      <c r="F39" s="23" t="s">
+      <c r="F40" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="G39">
-        <v>1</v>
-      </c>
-      <c r="H39">
-        <v>1</v>
-      </c>
-      <c r="I39">
+      <c r="G40">
+        <v>1</v>
+      </c>
+      <c r="H40">
+        <v>1</v>
+      </c>
+      <c r="I40">
         <f t="shared" si="6"/>
         <v>1</v>
       </c>
-      <c r="J39" s="9">
+      <c r="J40" s="9">
         <v>14.43</v>
       </c>
-      <c r="K39" s="16">
-        <f>J39/H39</f>
+      <c r="K40" s="16">
+        <f>J40/H40</f>
         <v>14.43</v>
       </c>
-      <c r="L39" s="16">
-        <f t="shared" ref="L39" si="9">I39*J39</f>
+      <c r="L40" s="16">
+        <f t="shared" ref="L40" si="9">I40*J40</f>
         <v>14.43</v>
       </c>
-      <c r="N39" s="8"/>
+      <c r="N40" s="8"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D13" r:id="rId1" display="https://www.mouser.ca/manufacturer/koa-speer/" xr:uid="{47E96BD1-A58F-40D3-8CED-17C5D166F0B7}"/>
-    <hyperlink ref="D17" r:id="rId2" display="https://www.mouser.ca/manufacturer/koa-speer/" xr:uid="{3FAD2419-4B3D-4B11-8688-1A2CE5B6EA06}"/>
-    <hyperlink ref="D14" r:id="rId3" display="https://www.mouser.ca/manufacturer/koa-speer/" xr:uid="{82378215-6481-407F-BE48-FDF5CE4FFCC6}"/>
-    <hyperlink ref="D16" r:id="rId4" display="https://www.mouser.ca/manufacturer/koa-speer/" xr:uid="{6E7276E1-1FE8-43FE-BB56-480F0D290C4A}"/>
-    <hyperlink ref="D15" r:id="rId5" display="https://www.mouser.ca/manufacturer/koa-speer/" xr:uid="{CA2B9258-5951-4014-96C5-E0072FBB388A}"/>
+    <hyperlink ref="D14" r:id="rId1" display="https://www.mouser.ca/manufacturer/koa-speer/" xr:uid="{47E96BD1-A58F-40D3-8CED-17C5D166F0B7}"/>
+    <hyperlink ref="D18" r:id="rId2" display="https://www.mouser.ca/manufacturer/koa-speer/" xr:uid="{3FAD2419-4B3D-4B11-8688-1A2CE5B6EA06}"/>
+    <hyperlink ref="D15" r:id="rId3" display="https://www.mouser.ca/manufacturer/koa-speer/" xr:uid="{82378215-6481-407F-BE48-FDF5CE4FFCC6}"/>
+    <hyperlink ref="D17" r:id="rId4" display="https://www.mouser.ca/manufacturer/koa-speer/" xr:uid="{6E7276E1-1FE8-43FE-BB56-480F0D290C4A}"/>
+    <hyperlink ref="D16" r:id="rId5" display="https://www.mouser.ca/manufacturer/koa-speer/" xr:uid="{CA2B9258-5951-4014-96C5-E0072FBB388A}"/>
     <hyperlink ref="N5" r:id="rId6" xr:uid="{765A1CAF-EB76-4432-AA0B-18A1158BBFA5}"/>
     <hyperlink ref="N7" r:id="rId7" xr:uid="{147678BE-8808-466F-B8D0-CA509E0FBF10}"/>
     <hyperlink ref="N8" r:id="rId8" xr:uid="{839DC45B-4DF9-4BA3-935C-45F827D02468}"/>
@@ -2169,14 +2222,14 @@
     <hyperlink ref="N10" r:id="rId10" xr:uid="{026358CC-9D33-41A6-81E7-B762049646CA}"/>
     <hyperlink ref="N11" r:id="rId11" xr:uid="{F3907DA5-0615-4F45-93E4-32383D66B841}"/>
     <hyperlink ref="N12" r:id="rId12" xr:uid="{0BCE2FF9-E18C-44DA-9ACB-D5D9E13CBC7A}"/>
-    <hyperlink ref="N17" r:id="rId13" xr:uid="{330480F0-BAC1-41DA-A7B5-6DEADD42BA32}"/>
-    <hyperlink ref="N13" r:id="rId14" xr:uid="{DB5C664D-9345-4BDC-818A-A2AB6600F928}"/>
-    <hyperlink ref="N14" r:id="rId15" xr:uid="{C8B16F51-D560-4B17-9BC0-57EA634FE372}"/>
-    <hyperlink ref="N20" r:id="rId16" xr:uid="{009A33E6-BEF9-4CB6-BB1D-EAAE981220A3}"/>
-    <hyperlink ref="N18" r:id="rId17" xr:uid="{5B07E0C4-F399-4789-955C-1299DEDF2CC6}"/>
-    <hyperlink ref="N37" r:id="rId18" xr:uid="{0D694F14-4FF2-4DE3-A582-15544C157E78}"/>
-    <hyperlink ref="N15" r:id="rId19" xr:uid="{580984EB-24D5-4BB4-99EF-23EB323FDFB4}"/>
-    <hyperlink ref="N16" r:id="rId20" xr:uid="{E884F790-766A-4C38-9046-4F373E3627DB}"/>
+    <hyperlink ref="N18" r:id="rId13" xr:uid="{330480F0-BAC1-41DA-A7B5-6DEADD42BA32}"/>
+    <hyperlink ref="N14" r:id="rId14" xr:uid="{DB5C664D-9345-4BDC-818A-A2AB6600F928}"/>
+    <hyperlink ref="N15" r:id="rId15" xr:uid="{C8B16F51-D560-4B17-9BC0-57EA634FE372}"/>
+    <hyperlink ref="N21" r:id="rId16" xr:uid="{009A33E6-BEF9-4CB6-BB1D-EAAE981220A3}"/>
+    <hyperlink ref="N19" r:id="rId17" xr:uid="{5B07E0C4-F399-4789-955C-1299DEDF2CC6}"/>
+    <hyperlink ref="N38" r:id="rId18" xr:uid="{0D694F14-4FF2-4DE3-A582-15544C157E78}"/>
+    <hyperlink ref="N16" r:id="rId19" xr:uid="{580984EB-24D5-4BB4-99EF-23EB323FDFB4}"/>
+    <hyperlink ref="N17" r:id="rId20" xr:uid="{E884F790-766A-4C38-9046-4F373E3627DB}"/>
     <hyperlink ref="N6" r:id="rId21" xr:uid="{98DDF687-010F-45EC-9E4B-94A5F44E7921}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2185,21 +2238,19 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="72c39c84-b0a3-45a2-a38c-ff46bb47f11f" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="cf9f6c1f-8ad0-4eb8-bb2b-fb0b622a341e">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B51EC7ECFAC78D4E8EF6CBAFFF0B3505" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7e0d9d996845e2cef65e12e895c4c91e">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="cf9f6c1f-8ad0-4eb8-bb2b-fb0b622a341e" xmlns:ns3="72c39c84-b0a3-45a2-a38c-ff46bb47f11f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="97eb945ec045b4d52e9ff03a8a8db852" ns2:_="" ns3:_="">
-    <xsd:import namespace="cf9f6c1f-8ad0-4eb8-bb2b-fb0b622a341e"/>
-    <xsd:import namespace="72c39c84-b0a3-45a2-a38c-ff46bb47f11f"/>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001DC44D19606E8540AF995795CBBBCE63" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e7289f370a5204a7f65a57e64255ba54">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="e718a8af-5d48-45b1-a7fb-cef00c107a7a" xmlns:ns3="715913e6-4bf0-458f-8160-f18e142d04ff" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="dfa4d2400c415f2e6245c833fda60061" ns2:_="" ns3:_="">
+    <xsd:import namespace="e718a8af-5d48-45b1-a7fb-cef00c107a7a"/>
+    <xsd:import namespace="715913e6-4bf0-458f-8160-f18e142d04ff"/>
     <xsd:element name="properties">
       <xsd:complexType>
         <xsd:sequence>
@@ -2210,14 +2261,12 @@
                 <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceAutoKeyPoints" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceKeyPoints" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceLocation" minOccurs="0"/>
-                <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
-                <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
                 <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
                 <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
@@ -2228,7 +2277,7 @@
       </xsd:complexType>
     </xsd:element>
   </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="cf9f6c1f-8ad0-4eb8-bb2b-fb0b622a341e" elementFormDefault="qualified">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="e718a8af-5d48-45b1-a7fb-cef00c107a7a" elementFormDefault="qualified">
     <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
@@ -2253,81 +2302,55 @@
         </xsd:restriction>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaServiceDateTaken" ma:index="12" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+    <xsd:element name="MediaServiceGenerationTime" ma:index="12" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaServiceGenerationTime" ma:index="13" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+    <xsd:element name="MediaServiceEventHashCode" ma:index="13" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaServiceEventHashCode" ma:index="14" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceOCR" ma:index="15" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+    <xsd:element name="MediaServiceOCR" ma:index="14" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note">
           <xsd:maxLength value="255"/>
         </xsd:restriction>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaServiceLocation" ma:index="16" nillable="true" ma:displayName="Location" ma:internalName="MediaServiceLocation" ma:readOnly="true">
+    <xsd:element name="MediaServiceDateTaken" ma:index="15" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaLengthInSeconds" ma:index="19" nillable="true" ma:displayName="Length (seconds)" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
+    <xsd:element name="MediaLengthInSeconds" ma:index="16" nillable="true" ma:displayName="MediaLengthInSeconds" ma:hidden="true" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Unknown"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="21" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="26ec1fed-e6ae-4c84-a4ac-123136fd9316" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+    <xsd:element name="MediaServiceLocation" ma:index="17" nillable="true" ma:displayName="Location" ma:internalName="MediaServiceLocation" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="19" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="26ec1fed-e6ae-4c84-a4ac-123136fd9316" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
       <xsd:complexType>
         <xsd:sequence>
           <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
         </xsd:sequence>
       </xsd:complexType>
     </xsd:element>
-    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="23" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:description="" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
+    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="21" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:description="" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="72c39c84-b0a3-45a2-a38c-ff46bb47f11f" elementFormDefault="qualified">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="715913e6-4bf0-458f-8160-f18e142d04ff" elementFormDefault="qualified">
     <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="SharedWithUsers" ma:index="17" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:UserMulti">
-            <xsd:sequence>
-              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
-                <xsd:complexType>
-                  <xsd:sequence>
-                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
-                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
-                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
-                  </xsd:sequence>
-                </xsd:complexType>
-              </xsd:element>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="SharedWithDetails" ma:index="18" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="TaxCatchAll" ma:index="22" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{230263d0-9f1a-4e63-a49c-f06b563fb00a}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="72c39c84-b0a3-45a2-a38c-ff46bb47f11f">
+    <xsd:element name="TaxCatchAll" ma:index="20" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{b05470fb-f248-421d-a4ae-c1bb0b45488d}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="715913e6-4bf0-458f-8160-f18e142d04ff">
       <xsd:complexType>
         <xsd:complexContent>
           <xsd:extension base="dms:MultiChoiceLookup">
@@ -2439,34 +2462,33 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="715913e6-4bf0-458f-8160-f18e142d04ff" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="e718a8af-5d48-45b1-a7fb-cef00c107a7a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4958292-C6C4-482B-887A-6CF9FB19AB74}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4740145F-09D2-466B-B9A2-2798696B0ADF}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="72c39c84-b0a3-45a2-a38c-ff46bb47f11f"/>
-    <ds:schemaRef ds:uri="cf9f6c1f-8ad0-4eb8-bb2b-fb0b622a341e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{01E2E549-AE8A-46C8-A391-10CE0BB53EF2}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A4A5C8E9-1634-4C66-8DF7-316C74B8FA24}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
     <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="cf9f6c1f-8ad0-4eb8-bb2b-fb0b622a341e"/>
-    <ds:schemaRef ds:uri="72c39c84-b0a3-45a2-a38c-ff46bb47f11f"/>
+    <ds:schemaRef ds:uri="e718a8af-5d48-45b1-a7fb-cef00c107a7a"/>
+    <ds:schemaRef ds:uri="715913e6-4bf0-458f-8160-f18e142d04ff"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
@@ -2478,9 +2500,14 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4740145F-09D2-466B-B9A2-2798696B0ADF}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4958292-C6C4-482B-887A-6CF9FB19AB74}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="72c39c84-b0a3-45a2-a38c-ff46bb47f11f"/>
+    <ds:schemaRef ds:uri="cf9f6c1f-8ad0-4eb8-bb2b-fb0b622a341e"/>
+    <ds:schemaRef ds:uri="715913e6-4bf0-458f-8160-f18e142d04ff"/>
+    <ds:schemaRef ds:uri="e718a8af-5d48-45b1-a7fb-cef00c107a7a"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>